<commit_message>
add sample database design
</commit_message>
<xml_diff>
--- a/Database Structure.xlsx
+++ b/Database Structure.xlsx
@@ -5,15 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SIMS\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SIMS\docs\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10365" windowHeight="4335" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10365" windowHeight="4335" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="1" r:id="rId1"/>
     <sheet name="student" sheetId="2" r:id="rId2"/>
+    <sheet name="Course-Units" sheetId="3" r:id="rId3"/>
+    <sheet name="MajorCousce" sheetId="7" r:id="rId4"/>
+    <sheet name="Grade" sheetId="4" r:id="rId5"/>
+    <sheet name="Teacher" sheetId="5" r:id="rId6"/>
+    <sheet name="ClassSheduling" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet6" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet7" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
   <si>
     <t>Person00</t>
   </si>
@@ -91,12 +98,6 @@
   </si>
   <si>
     <t>A-2</t>
-  </si>
-  <si>
-    <t>Student01</t>
-  </si>
-  <si>
-    <t>including classroom</t>
   </si>
   <si>
     <t>Person01id</t>
@@ -576,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +607,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -632,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -658,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -684,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -715,22 +716,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>4</v>
@@ -747,16 +748,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E9">
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G9" s="2">
         <v>42808</v>
@@ -773,16 +774,16 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G10" s="2">
         <v>42808</v>
@@ -799,16 +800,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
       <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
         <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>41</v>
       </c>
       <c r="G11" s="2">
         <v>42808</v>
@@ -825,16 +826,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>36</v>
       </c>
-      <c r="E12" t="s">
-        <v>38</v>
-      </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G12" s="2">
         <v>42808</v>
@@ -851,16 +852,16 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
-      </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G13" s="2">
         <v>42808</v>
@@ -877,16 +878,16 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G14" s="2">
         <v>42808</v>
@@ -903,16 +904,16 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G15" s="2">
         <v>42808</v>
@@ -929,16 +930,16 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
         <v>51</v>
       </c>
-      <c r="D16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" t="s">
-        <v>53</v>
-      </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G16" s="2">
         <v>42808</v>
@@ -955,16 +956,16 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E17" s="2">
         <v>33604</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G17" s="2">
         <v>42808</v>
@@ -981,16 +982,16 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
         <v>56</v>
       </c>
-      <c r="D18" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" t="s">
-        <v>58</v>
-      </c>
       <c r="F18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G18" s="2">
         <v>42808</v>
@@ -1007,16 +1008,16 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G19" s="2">
         <v>42808</v>
@@ -1036,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1148,7 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F5" s="2">
         <v>42736</v>
@@ -1157,17 +1158,97 @@
       </c>
       <c r="H5">
         <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>